<commit_message>
added facility for consducting election for any no of positions
</commit_message>
<xml_diff>
--- a/candidates_sample.xlsx
+++ b/candidates_sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t xml:space="preserve">ROLLNO</t>
   </si>
@@ -101,6 +101,21 @@
   </si>
   <si>
     <t xml:space="preserve">SURAJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B180010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">appukutan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entho secretary</t>
   </si>
 </sst>
 </file>
@@ -208,10 +223,10 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.28"/>
   </cols>
@@ -353,7 +368,21 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>

</xml_diff>